<commit_message>
Added new format for regions data as a factor variable
</commit_message>
<xml_diff>
--- a/Data files/Raw data files/country_regions2.xlsx
+++ b/Data files/Raw data files/country_regions2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timmyballesteros/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timmyballesteros/R/conflict-relapse/Data files/Raw data files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506136A8-1697-4448-AB22-B6AE1AD5EDAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8B2C44-F628-FF4E-BBB7-0CBB86E2375B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26000" windowHeight="17020" xr2:uid="{AB349C85-47AA-6640-986E-56E6FBE48942}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="26000" windowHeight="17020" xr2:uid="{AB349C85-47AA-6640-986E-56E6FBE48942}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -683,9 +683,6 @@
     <t>Central America</t>
   </si>
   <si>
-    <t>Carribean</t>
-  </si>
-  <si>
     <t>South America</t>
   </si>
   <si>
@@ -720,13 +717,16 @@
   </si>
   <si>
     <t>Southeast Asia</t>
+  </si>
+  <si>
+    <t>Caribbean</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -789,9 +789,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -829,7 +829,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -935,7 +935,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1077,7 +1077,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1089,12 +1089,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>101</v>
       </c>
@@ -1105,46 +1105,46 @@
         <v>214</v>
       </c>
       <c r="D1" t="s">
+        <v>227</v>
+      </c>
+      <c r="E1" t="s">
         <v>215</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>216</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>217</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>218</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>219</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>220</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>221</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>222</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>223</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>224</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>225</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>226</v>
       </c>
-      <c r="P1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>176</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="18">
+    <row r="3" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>104</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="18">
+    <row r="4" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>61</v>
       </c>
@@ -1170,7 +1170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="18">
+    <row r="5" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>177</v>
       </c>
@@ -1179,7 +1179,7 @@
       </c>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:16" ht="18">
+    <row r="6" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>105</v>
       </c>
@@ -1188,7 +1188,7 @@
       </c>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:16" ht="18">
+    <row r="7" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>178</v>
       </c>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:16" ht="18">
+    <row r="8" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>179</v>
       </c>
@@ -1206,7 +1206,7 @@
       </c>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:16" ht="18">
+    <row r="9" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>106</v>
       </c>
@@ -1215,7 +1215,7 @@
       </c>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:16" ht="18">
+    <row r="10" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -1224,7 +1224,7 @@
       </c>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:16" ht="18">
+    <row r="11" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>107</v>
       </c>
@@ -1233,7 +1233,7 @@
       </c>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:16" ht="18">
+    <row r="12" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>180</v>
       </c>
@@ -1242,7 +1242,7 @@
       </c>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:16" ht="18">
+    <row r="13" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>108</v>
       </c>
@@ -1251,7 +1251,7 @@
       </c>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:16" ht="18">
+    <row r="14" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>109</v>
       </c>
@@ -1260,7 +1260,7 @@
       </c>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:16" ht="18">
+    <row r="15" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>85</v>
       </c>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:16" ht="18">
+    <row r="16" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>41</v>
       </c>
@@ -1278,7 +1278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="18">
+    <row r="17" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>110</v>
       </c>
@@ -1287,7 +1287,7 @@
       </c>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:16" ht="18">
+    <row r="18" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>111</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="18">
+    <row r="19" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>71</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="18">
+    <row r="20" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>5</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="18">
+    <row r="21" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>112</v>
       </c>
@@ -1323,7 +1323,7 @@
       </c>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:16" ht="18">
+    <row r="22" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>113</v>
       </c>
@@ -1332,7 +1332,7 @@
       </c>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:16" ht="18">
+    <row r="23" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>181</v>
       </c>
@@ -1341,7 +1341,7 @@
       </c>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:16" ht="18">
+    <row r="24" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>86</v>
       </c>
@@ -1350,7 +1350,7 @@
       </c>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:16" ht="18">
+    <row r="25" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>114</v>
       </c>
@@ -1359,7 +1359,7 @@
       </c>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:16" ht="18">
+    <row r="26" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>182</v>
       </c>
@@ -1368,7 +1368,7 @@
       </c>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:16" ht="18">
+    <row r="27" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>21</v>
       </c>
@@ -1377,7 +1377,7 @@
       </c>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:16" ht="18">
+    <row r="28" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>115</v>
       </c>
@@ -1386,7 +1386,7 @@
       </c>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:16" ht="18">
+    <row r="29" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>183</v>
       </c>
@@ -1395,7 +1395,7 @@
       </c>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:16" ht="18">
+    <row r="30" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>116</v>
       </c>
@@ -1404,7 +1404,7 @@
       </c>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:16" ht="18">
+    <row r="31" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>119</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="18">
+    <row r="32" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>118</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="18">
+    <row r="33" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>117</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="18">
+    <row r="34" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>96</v>
       </c>
@@ -1440,7 +1440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="18">
+    <row r="35" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>120</v>
       </c>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="I35" s="2"/>
     </row>
-    <row r="36" spans="1:15" ht="18">
+    <row r="36" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>121</v>
       </c>
@@ -1458,7 +1458,7 @@
       </c>
       <c r="I36" s="2"/>
     </row>
-    <row r="37" spans="1:15" ht="18">
+    <row r="37" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>59</v>
       </c>
@@ -1467,7 +1467,7 @@
       </c>
       <c r="I37" s="2"/>
     </row>
-    <row r="38" spans="1:15" ht="18">
+    <row r="38" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>4</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="18">
+    <row r="39" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>99</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="18">
+    <row r="40" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>11</v>
       </c>
@@ -1494,7 +1494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="18">
+    <row r="41" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>36</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="18">
+    <row r="42" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>92</v>
       </c>
@@ -1512,7 +1512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="18">
+    <row r="43" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
@@ -1521,7 +1521,7 @@
       </c>
       <c r="I43" s="2"/>
     </row>
-    <row r="44" spans="1:15" ht="18">
+    <row r="44" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>72</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="18">
+    <row r="45" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>122</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="18">
+    <row r="46" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>26</v>
       </c>
@@ -1547,7 +1547,7 @@
       </c>
       <c r="I46" s="2"/>
     </row>
-    <row r="47" spans="1:15" ht="18">
+    <row r="47" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>31</v>
       </c>
@@ -1556,7 +1556,7 @@
       </c>
       <c r="I47" s="2"/>
     </row>
-    <row r="48" spans="1:15" ht="18">
+    <row r="48" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>123</v>
       </c>
@@ -1565,7 +1565,7 @@
       </c>
       <c r="I48" s="2"/>
     </row>
-    <row r="49" spans="1:9" ht="18">
+    <row r="49" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>124</v>
       </c>
@@ -1574,7 +1574,7 @@
       </c>
       <c r="I49" s="2"/>
     </row>
-    <row r="50" spans="1:9" ht="18">
+    <row r="50" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>125</v>
       </c>
@@ -1583,7 +1583,7 @@
       </c>
       <c r="I50" s="2"/>
     </row>
-    <row r="51" spans="1:9" ht="18">
+    <row r="51" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>126</v>
       </c>
@@ -1592,7 +1592,7 @@
       </c>
       <c r="I51" s="2"/>
     </row>
-    <row r="52" spans="1:9" ht="18">
+    <row r="52" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>80</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="18">
+    <row r="53" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>184</v>
       </c>
@@ -1609,7 +1609,7 @@
       </c>
       <c r="I53" s="2"/>
     </row>
-    <row r="54" spans="1:9" ht="18">
+    <row r="54" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>127</v>
       </c>
@@ -1618,7 +1618,7 @@
       </c>
       <c r="I54" s="2"/>
     </row>
-    <row r="55" spans="1:9" ht="18">
+    <row r="55" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>43</v>
       </c>
@@ -1627,7 +1627,7 @@
       </c>
       <c r="I55" s="2"/>
     </row>
-    <row r="56" spans="1:9" ht="18">
+    <row r="56" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>15</v>
       </c>
@@ -1636,7 +1636,7 @@
       </c>
       <c r="I56" s="2"/>
     </row>
-    <row r="57" spans="1:9" ht="18">
+    <row r="57" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>128</v>
       </c>
@@ -1645,7 +1645,7 @@
       </c>
       <c r="I57" s="2"/>
     </row>
-    <row r="58" spans="1:9" ht="18">
+    <row r="58" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>88</v>
       </c>
@@ -1654,7 +1654,7 @@
       </c>
       <c r="I58" s="2"/>
     </row>
-    <row r="59" spans="1:9" ht="18">
+    <row r="59" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>60</v>
       </c>
@@ -1662,7 +1662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="18">
+    <row r="60" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>185</v>
       </c>
@@ -1671,7 +1671,7 @@
       </c>
       <c r="I60" s="2"/>
     </row>
-    <row r="61" spans="1:9" ht="18">
+    <row r="61" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>66</v>
       </c>
@@ -1680,7 +1680,7 @@
       </c>
       <c r="I61" s="2"/>
     </row>
-    <row r="62" spans="1:9" ht="18">
+    <row r="62" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>129</v>
       </c>
@@ -1689,7 +1689,7 @@
       </c>
       <c r="I62" s="2"/>
     </row>
-    <row r="63" spans="1:9" ht="18">
+    <row r="63" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>6</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="18">
+    <row r="64" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>130</v>
       </c>
@@ -1706,7 +1706,7 @@
       </c>
       <c r="I64" s="2"/>
     </row>
-    <row r="65" spans="1:16" ht="18">
+    <row r="65" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>131</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:16" ht="18">
+    <row r="66" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>38</v>
       </c>
@@ -1724,7 +1724,7 @@
       </c>
       <c r="I66" s="2"/>
     </row>
-    <row r="67" spans="1:16" ht="18">
+    <row r="67" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>186</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:16" ht="18">
+    <row r="68" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>40</v>
       </c>
@@ -1742,7 +1742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:16" ht="18">
+    <row r="69" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>55</v>
       </c>
@@ -1751,7 +1751,7 @@
       </c>
       <c r="I69" s="2"/>
     </row>
-    <row r="70" spans="1:16" ht="18">
+    <row r="70" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>81</v>
       </c>
@@ -1760,7 +1760,7 @@
       </c>
       <c r="I70" s="2"/>
     </row>
-    <row r="71" spans="1:16" ht="18">
+    <row r="71" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>45</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:16" ht="18">
+    <row r="72" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>49</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:16" ht="18">
+    <row r="73" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>67</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:16" ht="18">
+    <row r="74" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>93</v>
       </c>
@@ -1796,7 +1796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:16" ht="18">
+    <row r="75" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>132</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:16" ht="18">
+    <row r="76" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>22</v>
       </c>
@@ -1814,7 +1814,7 @@
       </c>
       <c r="I76" s="2"/>
     </row>
-    <row r="77" spans="1:16" ht="18">
+    <row r="77" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>187</v>
       </c>
@@ -1823,7 +1823,7 @@
       </c>
       <c r="I77" s="2"/>
     </row>
-    <row r="78" spans="1:16" ht="18">
+    <row r="78" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>27</v>
       </c>
@@ -1832,7 +1832,7 @@
       </c>
       <c r="I78" s="2"/>
     </row>
-    <row r="79" spans="1:16" ht="18">
+    <row r="79" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>188</v>
       </c>
@@ -1841,7 +1841,7 @@
       </c>
       <c r="I79" s="2"/>
     </row>
-    <row r="80" spans="1:16" ht="18">
+    <row r="80" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>133</v>
       </c>
@@ -1850,7 +1850,7 @@
       </c>
       <c r="I80" s="2"/>
     </row>
-    <row r="81" spans="1:16" ht="18">
+    <row r="81" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>189</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:16" ht="18">
+    <row r="82" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>134</v>
       </c>
@@ -1868,7 +1868,7 @@
       </c>
       <c r="I82" s="2"/>
     </row>
-    <row r="83" spans="1:16" ht="18">
+    <row r="83" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>87</v>
       </c>
@@ -1877,7 +1877,7 @@
       </c>
       <c r="I83" s="2"/>
     </row>
-    <row r="84" spans="1:16" ht="18">
+    <row r="84" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>82</v>
       </c>
@@ -1886,7 +1886,7 @@
       </c>
       <c r="I84" s="2"/>
     </row>
-    <row r="85" spans="1:16" ht="18">
+    <row r="85" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>135</v>
       </c>
@@ -1895,7 +1895,7 @@
       </c>
       <c r="I85" s="2"/>
     </row>
-    <row r="86" spans="1:16" ht="18">
+    <row r="86" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>29</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:16" ht="18">
+    <row r="87" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>0</v>
       </c>
@@ -1913,7 +1913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:16" ht="18">
+    <row r="88" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>136</v>
       </c>
@@ -1922,7 +1922,7 @@
       </c>
       <c r="I88" s="2"/>
     </row>
-    <row r="89" spans="1:16" ht="18">
+    <row r="89" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>19</v>
       </c>
@@ -1931,7 +1931,7 @@
       </c>
       <c r="I89" s="2"/>
     </row>
-    <row r="90" spans="1:16" ht="18">
+    <row r="90" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>34</v>
       </c>
@@ -1940,7 +1940,7 @@
       </c>
       <c r="I90" s="2"/>
     </row>
-    <row r="91" spans="1:16" ht="18">
+    <row r="91" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>190</v>
       </c>
@@ -1949,7 +1949,7 @@
       </c>
       <c r="I91" s="2"/>
     </row>
-    <row r="92" spans="1:16" ht="18">
+    <row r="92" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>28</v>
       </c>
@@ -1958,7 +1958,7 @@
       </c>
       <c r="I92" s="2"/>
     </row>
-    <row r="93" spans="1:16" ht="18">
+    <row r="93" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>137</v>
       </c>
@@ -1967,7 +1967,7 @@
       </c>
       <c r="I93" s="2"/>
     </row>
-    <row r="94" spans="1:16" ht="18">
+    <row r="94" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>138</v>
       </c>
@@ -1976,7 +1976,7 @@
       </c>
       <c r="I94" s="2"/>
     </row>
-    <row r="95" spans="1:16" ht="18">
+    <row r="95" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>16</v>
       </c>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="I95" s="2"/>
     </row>
-    <row r="96" spans="1:16" ht="18">
+    <row r="96" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>139</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:16" ht="18">
+    <row r="97" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>140</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:16" ht="18">
+    <row r="98" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>68</v>
       </c>
@@ -2011,7 +2011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:16" ht="18">
+    <row r="99" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>141</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:16" ht="18">
+    <row r="100" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>48</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:16" ht="18">
+    <row r="101" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>191</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:16" ht="18">
+    <row r="102" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>192</v>
       </c>
@@ -2047,7 +2047,7 @@
       </c>
       <c r="I102" s="2"/>
     </row>
-    <row r="103" spans="1:16" ht="18">
+    <row r="103" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>142</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:16" ht="18">
+    <row r="104" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>143</v>
       </c>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="I104" s="2"/>
     </row>
-    <row r="105" spans="1:16" ht="18">
+    <row r="105" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>144</v>
       </c>
@@ -2074,7 +2074,7 @@
       </c>
       <c r="I105" s="2"/>
     </row>
-    <row r="106" spans="1:16" ht="18">
+    <row r="106" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>35</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:16" ht="18">
+    <row r="107" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>14</v>
       </c>
@@ -2092,7 +2092,7 @@
       </c>
       <c r="I107" s="2"/>
     </row>
-    <row r="108" spans="1:16" ht="18">
+    <row r="108" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>65</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:16" ht="18">
+    <row r="109" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>2</v>
       </c>
@@ -2110,7 +2110,7 @@
       </c>
       <c r="I109" s="2"/>
     </row>
-    <row r="110" spans="1:16" ht="18">
+    <row r="110" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>193</v>
       </c>
@@ -2119,7 +2119,7 @@
       </c>
       <c r="I110" s="2"/>
     </row>
-    <row r="111" spans="1:16" ht="18">
+    <row r="111" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>194</v>
       </c>
@@ -2128,7 +2128,7 @@
       </c>
       <c r="I111" s="2"/>
     </row>
-    <row r="112" spans="1:16" ht="18">
+    <row r="112" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>53</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:16" ht="18">
+    <row r="113" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>94</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:16" ht="18">
+    <row r="114" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>145</v>
       </c>
@@ -2155,7 +2155,7 @@
       </c>
       <c r="I114" s="2"/>
     </row>
-    <row r="115" spans="1:16" ht="18">
+    <row r="115" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>146</v>
       </c>
@@ -2164,7 +2164,7 @@
       </c>
       <c r="I115" s="2"/>
     </row>
-    <row r="116" spans="1:16" ht="18">
+    <row r="116" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>147</v>
       </c>
@@ -2173,7 +2173,7 @@
       </c>
       <c r="I116" s="2"/>
     </row>
-    <row r="117" spans="1:16" ht="18">
+    <row r="117" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>195</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:16" ht="18">
+    <row r="118" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>51</v>
       </c>
@@ -2191,7 +2191,7 @@
       </c>
       <c r="I118" s="2"/>
     </row>
-    <row r="119" spans="1:16" ht="18">
+    <row r="119" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>196</v>
       </c>
@@ -2200,7 +2200,7 @@
       </c>
       <c r="I119" s="2"/>
     </row>
-    <row r="120" spans="1:16" ht="18">
+    <row r="120" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>89</v>
       </c>
@@ -2209,7 +2209,7 @@
       </c>
       <c r="I120" s="2"/>
     </row>
-    <row r="121" spans="1:16" ht="18">
+    <row r="121" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>50</v>
       </c>
@@ -2218,7 +2218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:16" ht="18">
+    <row r="122" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>197</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:16" ht="18">
+    <row r="123" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>91</v>
       </c>
@@ -2236,7 +2236,7 @@
       </c>
       <c r="I123" s="2"/>
     </row>
-    <row r="124" spans="1:16" ht="18">
+    <row r="124" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>198</v>
       </c>
@@ -2245,7 +2245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:16" ht="18">
+    <row r="125" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>97</v>
       </c>
@@ -2254,7 +2254,7 @@
       </c>
       <c r="I125" s="2"/>
     </row>
-    <row r="126" spans="1:16" ht="18">
+    <row r="126" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>3</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:16" ht="18">
+    <row r="127" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>199</v>
       </c>
@@ -2272,7 +2272,7 @@
       </c>
       <c r="I127" s="2"/>
     </row>
-    <row r="128" spans="1:16" ht="18">
+    <row r="128" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>7</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:16" ht="18">
+    <row r="129" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>148</v>
       </c>
@@ -2290,7 +2290,7 @@
       </c>
       <c r="I129" s="2"/>
     </row>
-    <row r="130" spans="1:16" ht="18">
+    <row r="130" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>149</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:16" ht="18">
+    <row r="131" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>62</v>
       </c>
@@ -2308,7 +2308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:16" ht="18">
+    <row r="132" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>100</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:16" ht="18">
+    <row r="133" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>150</v>
       </c>
@@ -2325,7 +2325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:16" ht="18">
+    <row r="134" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>172</v>
       </c>
@@ -2334,7 +2334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:16" ht="18">
+    <row r="135" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>8</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:16" ht="18">
+    <row r="136" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>151</v>
       </c>
@@ -2352,7 +2352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:16" ht="18">
+    <row r="137" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>76</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:16" ht="18">
+    <row r="138" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>46</v>
       </c>
@@ -2370,7 +2370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:16" ht="18">
+    <row r="139" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>63</v>
       </c>
@@ -2379,7 +2379,7 @@
       </c>
       <c r="I139" s="2"/>
     </row>
-    <row r="140" spans="1:16" ht="18">
+    <row r="140" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>200</v>
       </c>
@@ -2388,7 +2388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:16" ht="18">
+    <row r="141" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>152</v>
       </c>
@@ -2397,7 +2397,7 @@
       </c>
       <c r="I141" s="2"/>
     </row>
-    <row r="142" spans="1:16" ht="18">
+    <row r="142" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>153</v>
       </c>
@@ -2406,7 +2406,7 @@
       </c>
       <c r="I142" s="2"/>
     </row>
-    <row r="143" spans="1:16" ht="18">
+    <row r="143" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>37</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:16" ht="18">
+    <row r="144" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>201</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:16" ht="18">
+    <row r="145" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>154</v>
       </c>
@@ -2433,7 +2433,7 @@
       </c>
       <c r="I145" s="2"/>
     </row>
-    <row r="146" spans="1:16" ht="18">
+    <row r="146" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>33</v>
       </c>
@@ -2442,7 +2442,7 @@
       </c>
       <c r="I146" s="2"/>
     </row>
-    <row r="147" spans="1:16" ht="18">
+    <row r="147" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>52</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:16" ht="18">
+    <row r="148" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>73</v>
       </c>
@@ -2460,7 +2460,7 @@
       </c>
       <c r="I148" s="2"/>
     </row>
-    <row r="149" spans="1:16" ht="18">
+    <row r="149" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>44</v>
       </c>
@@ -2469,7 +2469,7 @@
       </c>
       <c r="I149" s="2"/>
     </row>
-    <row r="150" spans="1:16" ht="18">
+    <row r="150" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>23</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:16" ht="18">
+    <row r="151" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>202</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:16" ht="18">
+    <row r="152" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>74</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:16" ht="18">
+    <row r="153" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>155</v>
       </c>
@@ -2505,7 +2505,7 @@
       </c>
       <c r="I153" s="2"/>
     </row>
-    <row r="154" spans="1:16" ht="18">
+    <row r="154" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>156</v>
       </c>
@@ -2514,7 +2514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:16" ht="18">
+    <row r="155" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>157</v>
       </c>
@@ -2523,7 +2523,7 @@
       </c>
       <c r="I155" s="2"/>
     </row>
-    <row r="156" spans="1:16" ht="18">
+    <row r="156" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>25</v>
       </c>
@@ -2532,7 +2532,7 @@
       </c>
       <c r="I156" s="2"/>
     </row>
-    <row r="157" spans="1:16" ht="18">
+    <row r="157" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>158</v>
       </c>
@@ -2541,7 +2541,7 @@
       </c>
       <c r="I157" s="2"/>
     </row>
-    <row r="158" spans="1:16" ht="18">
+    <row r="158" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>159</v>
       </c>
@@ -2550,7 +2550,7 @@
       </c>
       <c r="I158" s="2"/>
     </row>
-    <row r="159" spans="1:16" ht="18">
+    <row r="159" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>75</v>
       </c>
@@ -2559,7 +2559,7 @@
       </c>
       <c r="I159" s="2"/>
     </row>
-    <row r="160" spans="1:16" ht="18">
+    <row r="160" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>24</v>
       </c>
@@ -2568,7 +2568,7 @@
       </c>
       <c r="I160" s="2"/>
     </row>
-    <row r="161" spans="1:16" ht="18">
+    <row r="161" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>160</v>
       </c>
@@ -2577,7 +2577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:16" ht="18">
+    <row r="162" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>77</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:16" ht="18">
+    <row r="163" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>64</v>
       </c>
@@ -2595,7 +2595,7 @@
       </c>
       <c r="I163" s="2"/>
     </row>
-    <row r="164" spans="1:16" ht="18">
+    <row r="164" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>1</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:16" ht="18">
+    <row r="165" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>78</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:16" ht="18">
+    <row r="166" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>161</v>
       </c>
@@ -2621,7 +2621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:16" ht="18">
+    <row r="167" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>162</v>
       </c>
@@ -2630,7 +2630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:16" ht="18">
+    <row r="168" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>83</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:16" ht="18">
+    <row r="169" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>56</v>
       </c>
@@ -2648,7 +2648,7 @@
       </c>
       <c r="I169" s="2"/>
     </row>
-    <row r="170" spans="1:16" ht="18">
+    <row r="170" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>203</v>
       </c>
@@ -2657,7 +2657,7 @@
       </c>
       <c r="I170" s="2"/>
     </row>
-    <row r="171" spans="1:16" ht="18">
+    <row r="171" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>18</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:16" ht="18">
+    <row r="172" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>174</v>
       </c>
@@ -2674,7 +2674,7 @@
       </c>
       <c r="I172" s="2"/>
     </row>
-    <row r="173" spans="1:16" ht="18">
+    <row r="173" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>103</v>
       </c>
@@ -2683,7 +2683,7 @@
       </c>
       <c r="I173" s="2"/>
     </row>
-    <row r="174" spans="1:16" ht="18">
+    <row r="174" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>204</v>
       </c>
@@ -2692,7 +2692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:16" ht="18">
+    <row r="175" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>69</v>
       </c>
@@ -2701,7 +2701,7 @@
       </c>
       <c r="I175" s="2"/>
     </row>
-    <row r="176" spans="1:16" ht="18">
+    <row r="176" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>164</v>
       </c>
@@ -2710,7 +2710,7 @@
       </c>
       <c r="I176" s="2"/>
     </row>
-    <row r="177" spans="1:16" ht="18">
+    <row r="177" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>163</v>
       </c>
@@ -2719,7 +2719,7 @@
       </c>
       <c r="I177" s="2"/>
     </row>
-    <row r="178" spans="1:16" ht="18">
+    <row r="178" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>165</v>
       </c>
@@ -2728,7 +2728,7 @@
       </c>
       <c r="I178" s="2"/>
     </row>
-    <row r="179" spans="1:16" ht="18">
+    <row r="179" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>166</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:16" ht="18">
+    <row r="180" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>205</v>
       </c>
@@ -2745,7 +2745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:16" ht="18">
+    <row r="181" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
         <v>9</v>
       </c>
@@ -2754,7 +2754,7 @@
       </c>
       <c r="I181" s="2"/>
     </row>
-    <row r="182" spans="1:16" ht="18">
+    <row r="182" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>12</v>
       </c>
@@ -2763,7 +2763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:16" ht="18">
+    <row r="183" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
         <v>70</v>
       </c>
@@ -2772,7 +2772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:16" ht="18">
+    <row r="184" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>30</v>
       </c>
@@ -2781,7 +2781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:16" ht="18">
+    <row r="185" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
         <v>90</v>
       </c>
@@ -2790,7 +2790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:16" ht="18">
+    <row r="186" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>206</v>
       </c>
@@ -2799,7 +2799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:16" ht="18">
+    <row r="187" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
         <v>167</v>
       </c>
@@ -2808,7 +2808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:16" ht="18">
+    <row r="188" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
         <v>173</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:16" ht="18">
+    <row r="189" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
         <v>207</v>
       </c>
@@ -2826,7 +2826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:16" ht="18">
+    <row r="190" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
         <v>79</v>
       </c>
@@ -2835,7 +2835,7 @@
       </c>
       <c r="I190" s="2"/>
     </row>
-    <row r="191" spans="1:16" ht="18">
+    <row r="191" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
         <v>20</v>
       </c>
@@ -2844,7 +2844,7 @@
       </c>
       <c r="I191" s="2"/>
     </row>
-    <row r="192" spans="1:16" ht="18">
+    <row r="192" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
         <v>17</v>
       </c>
@@ -2853,7 +2853,7 @@
       </c>
       <c r="I192" s="2"/>
     </row>
-    <row r="193" spans="1:16" ht="18">
+    <row r="193" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
         <v>208</v>
       </c>
@@ -2862,7 +2862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:16" ht="18">
+    <row r="194" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
         <v>168</v>
       </c>
@@ -2871,7 +2871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:16" ht="18">
+    <row r="195" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
         <v>169</v>
       </c>
@@ -2879,7 +2879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:16" ht="18">
+    <row r="196" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
         <v>54</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:16" ht="18">
+    <row r="197" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
         <v>10</v>
       </c>
@@ -2896,7 +2896,7 @@
       </c>
       <c r="I197" s="2"/>
     </row>
-    <row r="198" spans="1:16" ht="18">
+    <row r="198" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
         <v>58</v>
       </c>
@@ -2905,7 +2905,7 @@
       </c>
       <c r="I198" s="2"/>
     </row>
-    <row r="199" spans="1:16" ht="18">
+    <row r="199" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
         <v>98</v>
       </c>
@@ -2914,7 +2914,7 @@
       </c>
       <c r="I199" s="2"/>
     </row>
-    <row r="200" spans="1:16" ht="18">
+    <row r="200" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
         <v>95</v>
       </c>
@@ -2923,7 +2923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:16" ht="18">
+    <row r="201" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
         <v>209</v>
       </c>
@@ -2932,7 +2932,7 @@
       </c>
       <c r="I201" s="2"/>
     </row>
-    <row r="202" spans="1:16" ht="18">
+    <row r="202" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
         <v>210</v>
       </c>
@@ -2941,7 +2941,7 @@
       </c>
       <c r="I202" s="2"/>
     </row>
-    <row r="203" spans="1:16" ht="18">
+    <row r="203" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
         <v>39</v>
       </c>
@@ -2950,7 +2950,7 @@
       </c>
       <c r="I203" s="2"/>
     </row>
-    <row r="204" spans="1:16" ht="18">
+    <row r="204" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
         <v>170</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:16" ht="18">
+    <row r="205" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
         <v>211</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:16" ht="18">
+    <row r="206" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
         <v>212</v>
       </c>
@@ -2977,7 +2977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:16" ht="18">
+    <row r="207" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
         <v>13</v>
       </c>
@@ -2986,7 +2986,7 @@
       </c>
       <c r="I207" s="2"/>
     </row>
-    <row r="208" spans="1:16" ht="18">
+    <row r="208" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
         <v>175</v>
       </c>
@@ -2995,7 +2995,7 @@
       </c>
       <c r="I208" s="2"/>
     </row>
-    <row r="209" spans="1:12" ht="18">
+    <row r="209" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
         <v>102</v>
       </c>
@@ -3004,7 +3004,7 @@
       </c>
       <c r="I209" s="2"/>
     </row>
-    <row r="210" spans="1:12" ht="18">
+    <row r="210" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
         <v>84</v>
       </c>
@@ -3013,7 +3013,7 @@
       </c>
       <c r="I210" s="2"/>
     </row>
-    <row r="211" spans="1:12" ht="18">
+    <row r="211" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
         <v>47</v>
       </c>
@@ -3022,7 +3022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:12" ht="18">
+    <row r="212" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
         <v>171</v>
       </c>
@@ -3031,7 +3031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:12" ht="18">
+    <row r="213" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
         <v>57</v>
       </c>
@@ -3040,76 +3040,76 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:12" ht="18">
+    <row r="214" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="I214" s="2"/>
     </row>
-    <row r="215" spans="1:12" ht="18">
+    <row r="215" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="I215" s="2"/>
     </row>
-    <row r="216" spans="1:12" ht="18">
+    <row r="216" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="I216" s="2"/>
     </row>
-    <row r="217" spans="1:12" ht="18">
+    <row r="217" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="I217" s="2"/>
     </row>
-    <row r="218" spans="1:12" ht="18">
+    <row r="218" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="I218" s="2"/>
     </row>
-    <row r="219" spans="1:12" ht="18">
+    <row r="219" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="I219" s="2"/>
     </row>
-    <row r="220" spans="1:12" ht="18">
+    <row r="220" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="I220" s="2"/>
     </row>
-    <row r="221" spans="1:12" ht="18">
+    <row r="221" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="I221" s="2"/>
     </row>
-    <row r="222" spans="1:12" ht="18">
+    <row r="222" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="I222" s="2"/>
     </row>
-    <row r="223" spans="1:12" ht="18">
+    <row r="223" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="I223" s="2"/>
     </row>
-    <row r="224" spans="1:12" ht="18">
+    <row r="224" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="I224" s="2"/>
     </row>
-    <row r="225" spans="9:9" ht="18">
+    <row r="225" spans="9:9" ht="18" x14ac:dyDescent="0.2">
       <c r="I225" s="2"/>
     </row>
-    <row r="226" spans="9:9" ht="18">
+    <row r="226" spans="9:9" ht="18" x14ac:dyDescent="0.2">
       <c r="I226" s="2"/>
     </row>
-    <row r="227" spans="9:9" ht="18">
+    <row r="227" spans="9:9" ht="18" x14ac:dyDescent="0.2">
       <c r="I227" s="2"/>
     </row>
-    <row r="228" spans="9:9" ht="18">
+    <row r="228" spans="9:9" ht="18" x14ac:dyDescent="0.2">
       <c r="I228" s="2"/>
     </row>
-    <row r="229" spans="9:9" ht="18">
+    <row r="229" spans="9:9" ht="18" x14ac:dyDescent="0.2">
       <c r="I229" s="2"/>
     </row>
-    <row r="230" spans="9:9" ht="18">
+    <row r="230" spans="9:9" ht="18" x14ac:dyDescent="0.2">
       <c r="I230" s="2"/>
     </row>
-    <row r="231" spans="9:9" ht="18">
+    <row r="231" spans="9:9" ht="18" x14ac:dyDescent="0.2">
       <c r="I231" s="2"/>
     </row>
-    <row r="232" spans="9:9" ht="18">
+    <row r="232" spans="9:9" ht="18" x14ac:dyDescent="0.2">
       <c r="I232" s="2"/>
     </row>
-    <row r="233" spans="9:9" ht="18">
+    <row r="233" spans="9:9" ht="18" x14ac:dyDescent="0.2">
       <c r="I233" s="2"/>
     </row>
-    <row r="234" spans="9:9" ht="18">
+    <row r="234" spans="9:9" ht="18" x14ac:dyDescent="0.2">
       <c r="I234" s="2"/>
     </row>
-    <row r="235" spans="9:9" ht="18">
+    <row r="235" spans="9:9" ht="18" x14ac:dyDescent="0.2">
       <c r="I235" s="2"/>
     </row>
-    <row r="236" spans="9:9" ht="18">
+    <row r="236" spans="9:9" ht="18" x14ac:dyDescent="0.2">
       <c r="I236" s="2"/>
     </row>
-    <row r="237" spans="9:9" ht="18">
+    <row r="237" spans="9:9" ht="18" x14ac:dyDescent="0.2">
       <c r="I237" s="2"/>
     </row>
   </sheetData>

</xml_diff>